<commit_message>
WIP command import from xlsx - first import complete
</commit_message>
<xml_diff>
--- a/assets/xlsx/Cod4.xlsx
+++ b/assets/xlsx/Cod4.xlsx
@@ -376,7 +376,7 @@
     <t>related_maps</t>
   </si>
   <si>
-    <t>order</t>
+    <t>number</t>
   </si>
   <si>
     <t>bonus_mission</t>
@@ -6253,7 +6253,7 @@
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>